<commit_message>
update: add timezone on database
</commit_message>
<xml_diff>
--- a/internal/service/stock/Customer All PB GROUP (Wilayah).xlsx
+++ b/internal/service/stock/Customer All PB GROUP (Wilayah).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\go\src\stock\internal\service\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F6B519-C27E-4B45-964C-E1B6AD795143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF4C570-7837-4FFB-AB8E-C472018EDA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10635" windowHeight="10920" firstSheet="8" activeTab="9" xr2:uid="{367E69BF-2037-4A2D-B60B-4D531090D608}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{367E69BF-2037-4A2D-B60B-4D531090D608}"/>
   </bookViews>
   <sheets>
     <sheet name="Risanto (0)" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10555" uniqueCount="6833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10556" uniqueCount="6834">
   <si>
     <t>BPR Karya Bakti Sejahtera</t>
   </si>
@@ -20567,6 +20567,9 @@
   </si>
   <si>
     <t>PBM-493</t>
+  </si>
+  <si>
+    <t>T. Samuel</t>
   </si>
 </sst>
 </file>
@@ -20748,7 +20751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -20833,6 +20836,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21462,8 +21489,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23037,7 +23064,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="F10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -23716,7 +23743,7 @@
         <v>5346</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -24244,7 +24271,7 @@
         <v>5346</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -24376,7 +24403,7 @@
         <v>5346</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -29683,7 +29710,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I56"/>
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31553,11 +31580,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC32A0D-2FF7-4C84-B3BE-EE2111149BE2}">
-  <sheetPr codeName="Sheet15"/>
+  <sheetPr codeName="Sheet15">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31566,10 +31595,10 @@
     <col min="2" max="2" width="21.5703125" style="15" customWidth="1"/>
     <col min="3" max="4" width="23.85546875" style="15"/>
     <col min="5" max="5" width="13.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="15" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="29" customWidth="1"/>
     <col min="10" max="16384" width="23.85546875" style="15"/>
   </cols>
   <sheetData>
@@ -31589,7 +31618,7 @@
       <c r="E1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="36" t="s">
         <v>151</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -31618,7 +31647,7 @@
       <c r="E2" s="3" t="s">
         <v>1789</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="37" t="s">
         <v>5763</v>
       </c>
       <c r="G2" s="2">
@@ -31651,7 +31680,7 @@
       <c r="E3" s="3" t="s">
         <v>1792</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="37" t="s">
         <v>5764</v>
       </c>
       <c r="G3" s="2">
@@ -31684,7 +31713,7 @@
       <c r="E4" s="3" t="s">
         <v>1795</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="37" t="s">
         <v>5765</v>
       </c>
       <c r="G4" s="2">
@@ -31717,7 +31746,7 @@
       <c r="E5" s="3" t="s">
         <v>1799</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="37" t="s">
         <v>5766</v>
       </c>
       <c r="G5" s="2">
@@ -31750,7 +31779,7 @@
       <c r="E6" s="3" t="s">
         <v>1802</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="37" t="s">
         <v>5767</v>
       </c>
       <c r="G6" s="2">
@@ -31783,7 +31812,7 @@
       <c r="E7" s="3" t="s">
         <v>1805</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="37" t="s">
         <v>5768</v>
       </c>
       <c r="G7" s="2">
@@ -31816,7 +31845,7 @@
       <c r="E8" s="3" t="s">
         <v>1808</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="37" t="s">
         <v>5769</v>
       </c>
       <c r="G8" s="2">
@@ -31849,7 +31878,7 @@
       <c r="E9" s="3" t="s">
         <v>1811</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="37" t="s">
         <v>5770</v>
       </c>
       <c r="G9" s="2">
@@ -31882,7 +31911,7 @@
       <c r="E10" s="3" t="s">
         <v>1814</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="37" t="s">
         <v>5771</v>
       </c>
       <c r="G10" s="2">
@@ -31915,7 +31944,7 @@
       <c r="E11" s="3" t="s">
         <v>1817</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="37" t="s">
         <v>5772</v>
       </c>
       <c r="G11" s="2">
@@ -31948,7 +31977,7 @@
       <c r="E12" s="3" t="s">
         <v>1820</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="37" t="s">
         <v>5773</v>
       </c>
       <c r="G12" s="2">
@@ -31981,7 +32010,7 @@
       <c r="E13" s="3" t="s">
         <v>1823</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="37" t="s">
         <v>5774</v>
       </c>
       <c r="G13" s="2">
@@ -32014,7 +32043,7 @@
       <c r="E14" s="3" t="s">
         <v>1825</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="37" t="s">
         <v>5775</v>
       </c>
       <c r="G14" s="2">
@@ -32047,7 +32076,7 @@
       <c r="E15" s="3" t="s">
         <v>1827</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="37" t="s">
         <v>5776</v>
       </c>
       <c r="G15" s="2">
@@ -32080,7 +32109,7 @@
       <c r="E16" s="3" t="s">
         <v>1830</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="37" t="s">
         <v>5777</v>
       </c>
       <c r="G16" s="2">
@@ -32113,7 +32142,7 @@
       <c r="E17" s="3" t="s">
         <v>1833</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="37" t="s">
         <v>5778</v>
       </c>
       <c r="G17" s="2">
@@ -32146,7 +32175,7 @@
       <c r="E18" s="3" t="s">
         <v>1837</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="37" t="s">
         <v>5779</v>
       </c>
       <c r="G18" s="2">
@@ -32179,7 +32208,7 @@
       <c r="E19" s="3" t="s">
         <v>1840</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="37" t="s">
         <v>5780</v>
       </c>
       <c r="G19" s="2">
@@ -32212,7 +32241,7 @@
       <c r="E20" s="3" t="s">
         <v>1843</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="37" t="s">
         <v>5781</v>
       </c>
       <c r="G20" s="2">
@@ -32245,7 +32274,7 @@
       <c r="E21" s="3" t="s">
         <v>1847</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="37" t="s">
         <v>5782</v>
       </c>
       <c r="G21" s="2">
@@ -32278,7 +32307,7 @@
       <c r="E22" s="3" t="s">
         <v>1851</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="37" t="s">
         <v>5783</v>
       </c>
       <c r="G22" s="2">
@@ -32311,7 +32340,7 @@
       <c r="E23" s="3" t="s">
         <v>1853</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="37" t="s">
         <v>5784</v>
       </c>
       <c r="G23" s="2">
@@ -32342,7 +32371,7 @@
         <v>19</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="37" t="s">
         <v>5785</v>
       </c>
       <c r="G24" s="2">
@@ -32375,7 +32404,7 @@
       <c r="E25" s="3" t="s">
         <v>1856</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="37" t="s">
         <v>5786</v>
       </c>
       <c r="G25" s="2">
@@ -32408,7 +32437,7 @@
       <c r="E26" s="3" t="s">
         <v>1859</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="37" t="s">
         <v>5787</v>
       </c>
       <c r="G26" s="2">
@@ -32441,7 +32470,7 @@
       <c r="E27" s="3" t="s">
         <v>1862</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="37" t="s">
         <v>5788</v>
       </c>
       <c r="G27" s="2">
@@ -32474,7 +32503,7 @@
       <c r="E28" s="3" t="s">
         <v>1865</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="37" t="s">
         <v>5789</v>
       </c>
       <c r="G28" s="2">
@@ -32507,7 +32536,7 @@
       <c r="E29" s="3" t="s">
         <v>1868</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="37" t="s">
         <v>5790</v>
       </c>
       <c r="G29" s="2">
@@ -32540,7 +32569,7 @@
       <c r="E30" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="37" t="s">
         <v>5791</v>
       </c>
       <c r="G30" s="2">
@@ -32573,7 +32602,7 @@
       <c r="E31" s="3" t="s">
         <v>1873</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="37" t="s">
         <v>5792</v>
       </c>
       <c r="G31" s="2">
@@ -32606,7 +32635,7 @@
       <c r="E32" s="3" t="s">
         <v>1876</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="37" t="s">
         <v>5793</v>
       </c>
       <c r="G32" s="2">
@@ -32639,7 +32668,7 @@
       <c r="E33" s="3" t="s">
         <v>1880</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="37" t="s">
         <v>5794</v>
       </c>
       <c r="G33" s="2">
@@ -32672,7 +32701,7 @@
       <c r="E34" s="3" t="s">
         <v>1883</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="37" t="s">
         <v>5795</v>
       </c>
       <c r="G34" s="2">
@@ -32705,7 +32734,7 @@
       <c r="E35" s="3" t="s">
         <v>1886</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="37" t="s">
         <v>5796</v>
       </c>
       <c r="G35" s="2">
@@ -32870,7 +32899,7 @@
       <c r="E40" s="3" t="s">
         <v>1901</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="37" t="s">
         <v>5801</v>
       </c>
       <c r="G40" s="2">
@@ -32903,7 +32932,7 @@
       <c r="E41" s="3" t="s">
         <v>1904</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="37" t="s">
         <v>5802</v>
       </c>
       <c r="G41" s="2">
@@ -33101,7 +33130,7 @@
       <c r="E47" s="3">
         <v>166678</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="37" t="s">
         <v>5808</v>
       </c>
       <c r="G47" s="2">
@@ -33134,7 +33163,7 @@
       <c r="E48" s="3" t="s">
         <v>1927</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="37" t="s">
         <v>5809</v>
       </c>
       <c r="G48" s="2">
@@ -33167,7 +33196,7 @@
       <c r="E49" s="3">
         <v>162278</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="37" t="s">
         <v>5810</v>
       </c>
       <c r="G49" s="2">
@@ -33189,7 +33218,8 @@
   <conditionalFormatting sqref="I2:I49">
     <cfRule type="uniqueValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.31496062992125984" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -39890,11 +39920,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22051960-1B52-4758-A191-518CA389CF85}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I46"/>
+  <sheetPr codeName="Sheet2">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39911,1531 +39943,1547 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="35" t="s">
+        <v>6833</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="32" t="s">
         <v>5147</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I2" s="33" t="s">
         <v>5148</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D3" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="36" t="s">
         <v>5155</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G3" s="31">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="str">
-        <f>IF(G2=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G2, 1) + 23, "000000"),
- IF(G2=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G2, 2) + 11, "000000"),
- IF(G2=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G2, 3) + 12, "000000"),
+      <c r="H3" s="32" t="str">
+        <f>IF(G3=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G3, 1) + 23, "000000"),
+ IF(G3=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G3, 2) + 11, "000000"),
+ IF(G3=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G3, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000024</v>
       </c>
-      <c r="I2" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="I3" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D4" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="36" t="s">
         <v>5156</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="31">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="str">
-        <f>IF(G3=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G3, 1) + 23, "000000"),
- IF(G3=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G3, 2) + 11, "000000"),
- IF(G3=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G3, 3) + 12, "000000"),
+      <c r="H4" s="32" t="str">
+        <f>IF(G4=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G4, 1) + 23, "000000"),
+ IF(G4=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G4, 2) + 11, "000000"),
+ IF(G4=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G4, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000025</v>
       </c>
-      <c r="I3" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="I4" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D5" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="31" t="s">
         <v>5157</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="31">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="str">
-        <f>IF(G4=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G4, 1) + 23, "000000"),
- IF(G4=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G4, 2) + 11, "000000"),
- IF(G4=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G4, 3) + 12, "000000"),
+      <c r="H5" s="32" t="str">
+        <f>IF(G5=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G5, 1) + 23, "000000"),
+ IF(G5=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G5, 2) + 11, "000000"),
+ IF(G5=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G5, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000026</v>
       </c>
-      <c r="I4" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="I5" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="31" t="s">
         <v>179</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="31" t="s">
         <v>5158</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G6" s="31">
         <v>1</v>
       </c>
-      <c r="H5" s="2" t="str">
-        <f>IF(G5=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G5, 1) + 23, "000000"),
- IF(G5=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G5, 2) + 11, "000000"),
- IF(G5=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G5, 3) + 12, "000000"),
+      <c r="H6" s="32" t="str">
+        <f>IF(G6=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G6, 1) + 23, "000000"),
+ IF(G6=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G6, 2) + 11, "000000"),
+ IF(G6=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G6, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000027</v>
       </c>
-      <c r="I5" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="I6" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="31" t="s">
         <v>5159</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G7" s="31">
         <v>1</v>
       </c>
-      <c r="H6" s="2" t="str">
-        <f>IF(G6=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G6, 1) + 23, "000000"),
- IF(G6=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G6, 2) + 11, "000000"),
- IF(G6=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G6, 3) + 12, "000000"),
+      <c r="H7" s="32" t="str">
+        <f>IF(G7=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G7, 1) + 23, "000000"),
+ IF(G7=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G7, 2) + 11, "000000"),
+ IF(G7=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G7, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000028</v>
       </c>
-      <c r="I6" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="I7" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="31" t="s">
         <v>5160</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G8" s="31">
         <v>2</v>
       </c>
-      <c r="H7" s="2" t="str">
-        <f>IF(G7=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G7, 1) + 23, "000000"),
- IF(G7=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G7, 2) + 11, "000000"),
- IF(G7=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G7, 3) + 12, "000000"),
+      <c r="H8" s="32" t="str">
+        <f>IF(G8=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G8, 1) + 23, "000000"),
+ IF(G8=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G8, 2) + 11, "000000"),
+ IF(G8=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G8, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000012</v>
       </c>
-      <c r="I7" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="I8" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="31" t="s">
         <v>5161</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="31">
         <v>2</v>
       </c>
-      <c r="H8" s="2" t="str">
-        <f>IF(G8=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G8, 1) + 23, "000000"),
- IF(G8=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G8, 2) + 11, "000000"),
- IF(G8=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G8, 3) + 12, "000000"),
+      <c r="H9" s="32" t="str">
+        <f>IF(G9=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G9, 1) + 23, "000000"),
+ IF(G9=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G9, 2) + 11, "000000"),
+ IF(G9=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G9, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000013</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="I9" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="31" t="s">
         <v>5162</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G10" s="31">
         <v>2</v>
       </c>
-      <c r="H9" s="2" t="str">
-        <f>IF(G9=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G9, 1) + 23, "000000"),
- IF(G9=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G9, 2) + 11, "000000"),
- IF(G9=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G9, 3) + 12, "000000"),
+      <c r="H10" s="32" t="str">
+        <f>IF(G10=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G10, 1) + 23, "000000"),
+ IF(G10=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G10, 2) + 11, "000000"),
+ IF(G10=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G10, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000014</v>
       </c>
-      <c r="I9" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="I10" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="31" t="s">
         <v>291</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="36" t="s">
         <v>5163</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G11" s="31">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="str">
-        <f>IF(G10=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G10, 1) + 23, "000000"),
- IF(G10=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G10, 2) + 11, "000000"),
- IF(G10=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G10, 3) + 12, "000000"),
+      <c r="H11" s="32" t="str">
+        <f>IF(G11=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G11, 1) + 23, "000000"),
+ IF(G11=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G11, 2) + 11, "000000"),
+ IF(G11=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G11, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000029</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="I11" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="36" t="s">
         <v>5164</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G12" s="31">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="str">
-        <f>IF(G11=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G11, 1) + 23, "000000"),
- IF(G11=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G11, 2) + 11, "000000"),
- IF(G11=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G11, 3) + 12, "000000"),
+      <c r="H12" s="32" t="str">
+        <f>IF(G12=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G12, 1) + 23, "000000"),
+ IF(G12=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G12, 2) + 11, "000000"),
+ IF(G12=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G12, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000030</v>
       </c>
-      <c r="I11" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="I12" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="36" t="s">
         <v>5165</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="31">
         <v>3</v>
       </c>
-      <c r="H12" s="2" t="str">
-        <f>IF(G12=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G12, 1) + 23, "000000"),
- IF(G12=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G12, 2) + 11, "000000"),
- IF(G12=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G12, 3) + 12, "000000"),
+      <c r="H13" s="32" t="str">
+        <f>IF(G13=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G13, 1) + 23, "000000"),
+ IF(G13=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G13, 2) + 11, "000000"),
+ IF(G13=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G13, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000013</v>
       </c>
-      <c r="I12" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="I13" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D14" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F14" s="31" t="s">
         <v>5166</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G14" s="31">
         <v>1</v>
       </c>
-      <c r="H13" s="2" t="str">
-        <f>IF(G13=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G13, 1) + 23, "000000"),
- IF(G13=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G13, 2) + 11, "000000"),
- IF(G13=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G13, 3) + 12, "000000"),
+      <c r="H14" s="32" t="str">
+        <f>IF(G14=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G14, 1) + 23, "000000"),
+ IF(G14=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G14, 2) + 11, "000000"),
+ IF(G14=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G14, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000031</v>
       </c>
-      <c r="I13" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="I14" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D15" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="31" t="s">
         <v>5167</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G15" s="31">
         <v>2</v>
       </c>
-      <c r="H14" s="2" t="str">
-        <f>IF(G14=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G14, 1) + 23, "000000"),
- IF(G14=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G14, 2) + 11, "000000"),
- IF(G14=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G14, 3) + 12, "000000"),
+      <c r="H15" s="32" t="str">
+        <f>IF(G15=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G15, 1) + 23, "000000"),
+ IF(G15=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G15, 2) + 11, "000000"),
+ IF(G15=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G15, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000015</v>
       </c>
-      <c r="I14" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="I15" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="31" t="s">
         <v>293</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D16" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="31" t="s">
         <v>5168</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G16" s="31">
         <v>1</v>
       </c>
-      <c r="H15" s="2" t="str">
-        <f>IF(G15=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G15, 1) + 23, "000000"),
- IF(G15=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G15, 2) + 11, "000000"),
- IF(G15=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G15, 3) + 12, "000000"),
+      <c r="H16" s="32" t="str">
+        <f>IF(G16=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G16, 1) + 23, "000000"),
+ IF(G16=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G16, 2) + 11, "000000"),
+ IF(G16=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G16, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000032</v>
       </c>
-      <c r="I15" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="I16" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F17" s="36" t="s">
         <v>5169</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G17" s="31">
         <v>1</v>
       </c>
-      <c r="H16" s="2" t="str">
-        <f>IF(G16=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G16, 1) + 23, "000000"),
- IF(G16=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G16, 2) + 11, "000000"),
- IF(G16=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G16, 3) + 12, "000000"),
+      <c r="H17" s="32" t="str">
+        <f>IF(G17=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G17, 1) + 23, "000000"),
+ IF(G17=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G17, 2) + 11, "000000"),
+ IF(G17=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G17, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000033</v>
       </c>
-      <c r="I16" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="I17" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="36" t="s">
         <v>5170</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G18" s="31">
         <v>3</v>
       </c>
-      <c r="H17" s="2" t="str">
-        <f>IF(G17=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G17, 1) + 23, "000000"),
- IF(G17=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G17, 2) + 11, "000000"),
- IF(G17=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G17, 3) + 12, "000000"),
+      <c r="H18" s="32" t="str">
+        <f>IF(G18=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G18, 1) + 23, "000000"),
+ IF(G18=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G18, 2) + 11, "000000"),
+ IF(G18=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G18, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000014</v>
       </c>
-      <c r="I17" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="I18" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D19" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F19" s="36" t="s">
         <v>5171</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G19" s="31">
         <v>3</v>
       </c>
-      <c r="H18" s="2" t="str">
-        <f>IF(G18=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G18, 1) + 23, "000000"),
- IF(G18=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G18, 2) + 11, "000000"),
- IF(G18=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G18, 3) + 12, "000000"),
+      <c r="H19" s="32" t="str">
+        <f>IF(G19=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G19, 1) + 23, "000000"),
+ IF(G19=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G19, 2) + 11, "000000"),
+ IF(G19=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G19, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000015</v>
       </c>
-      <c r="I18" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="I19" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F20" s="36" t="s">
         <v>5172</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="31">
         <v>1</v>
       </c>
-      <c r="H19" s="2" t="str">
-        <f>IF(G19=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G19, 1) + 23, "000000"),
- IF(G19=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G19, 2) + 11, "000000"),
- IF(G19=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G19, 3) + 12, "000000"),
+      <c r="H20" s="32" t="str">
+        <f>IF(G20=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G20, 1) + 23, "000000"),
+ IF(G20=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G20, 2) + 11, "000000"),
+ IF(G20=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G20, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000034</v>
       </c>
-      <c r="I19" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="I20" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="31" t="s">
         <v>5173</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G21" s="31">
         <v>3</v>
       </c>
-      <c r="H20" s="2" t="str">
-        <f>IF(G20=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G20, 1) + 23, "000000"),
- IF(G20=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G20, 2) + 11, "000000"),
- IF(G20=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G20, 3) + 12, "000000"),
+      <c r="H21" s="32" t="str">
+        <f>IF(G21=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G21, 1) + 23, "000000"),
+ IF(G21=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G21, 2) + 11, "000000"),
+ IF(G21=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G21, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000016</v>
       </c>
-      <c r="I20" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="I21" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D22" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E22" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F22" s="31" t="s">
         <v>5174</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G22" s="31">
         <v>2</v>
       </c>
-      <c r="H21" s="2" t="str">
-        <f>IF(G21=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G21, 1) + 23, "000000"),
- IF(G21=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G21, 2) + 11, "000000"),
- IF(G21=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G21, 3) + 12, "000000"),
+      <c r="H22" s="32" t="str">
+        <f>IF(G22=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G22, 1) + 23, "000000"),
+ IF(G22=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G22, 2) + 11, "000000"),
+ IF(G22=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G22, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000016</v>
       </c>
-      <c r="I21" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="I22" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D23" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F23" s="31" t="s">
         <v>5175</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G23" s="31">
         <v>3</v>
       </c>
-      <c r="H22" s="2" t="str">
-        <f>IF(G22=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G22, 1) + 23, "000000"),
- IF(G22=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G22, 2) + 11, "000000"),
- IF(G22=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G22, 3) + 12, "000000"),
+      <c r="H23" s="32" t="str">
+        <f>IF(G23=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G23, 1) + 23, "000000"),
+ IF(G23=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G23, 2) + 11, "000000"),
+ IF(G23=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G23, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000017</v>
       </c>
-      <c r="I22" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="I23" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="31" t="s">
         <v>5176</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G24" s="31">
         <v>1</v>
       </c>
-      <c r="H23" s="2" t="str">
-        <f>IF(G23=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G23, 1) + 23, "000000"),
- IF(G23=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G23, 2) + 11, "000000"),
- IF(G23=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G23, 3) + 12, "000000"),
+      <c r="H24" s="32" t="str">
+        <f>IF(G24=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G24, 1) + 23, "000000"),
+ IF(G24=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G24, 2) + 11, "000000"),
+ IF(G24=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G24, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000035</v>
       </c>
-      <c r="I23" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="I24" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="31">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="31" t="s">
         <v>5177</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G25" s="31">
         <v>1</v>
       </c>
-      <c r="H24" s="2" t="str">
-        <f>IF(G24=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G24, 1) + 23, "000000"),
- IF(G24=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G24, 2) + 11, "000000"),
- IF(G24=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G24, 3) + 12, "000000"),
+      <c r="H25" s="32" t="str">
+        <f>IF(G25=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G25, 1) + 23, "000000"),
+ IF(G25=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G25, 2) + 11, "000000"),
+ IF(G25=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G25, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000036</v>
       </c>
-      <c r="I24" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="I25" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="31">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D26" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="31" t="s">
         <v>5178</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G26" s="31">
         <v>2</v>
       </c>
-      <c r="H25" s="2" t="str">
-        <f>IF(G25=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G25, 1) + 23, "000000"),
- IF(G25=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G25, 2) + 11, "000000"),
- IF(G25=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G25, 3) + 12, "000000"),
+      <c r="H26" s="32" t="str">
+        <f>IF(G26=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G26, 1) + 23, "000000"),
+ IF(G26=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G26, 2) + 11, "000000"),
+ IF(G26=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G26, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000017</v>
       </c>
-      <c r="I25" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="I26" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="31">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F27" s="31" t="s">
         <v>5179</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G27" s="31">
         <v>3</v>
       </c>
-      <c r="H26" s="2" t="str">
-        <f>IF(G26=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G26, 1) + 23, "000000"),
- IF(G26=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G26, 2) + 11, "000000"),
- IF(G26=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G26, 3) + 12, "000000"),
+      <c r="H27" s="32" t="str">
+        <f>IF(G27=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G27, 1) + 23, "000000"),
+ IF(G27=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G27, 2) + 11, "000000"),
+ IF(G27=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G27, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000018</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="I27" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D28" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="31" t="s">
         <v>5180</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G28" s="31">
         <v>2</v>
       </c>
-      <c r="H27" s="2" t="str">
-        <f>IF(G27=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G27, 1) + 23, "000000"),
- IF(G27=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G27, 2) + 11, "000000"),
- IF(G27=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G27, 3) + 12, "000000"),
+      <c r="H28" s="32" t="str">
+        <f>IF(G28=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G28, 1) + 23, "000000"),
+ IF(G28=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G28, 2) + 11, "000000"),
+ IF(G28=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G28, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000018</v>
       </c>
-      <c r="I27" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="I28" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="31" t="s">
         <v>5181</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G29" s="31">
         <v>3</v>
       </c>
-      <c r="H28" s="2" t="str">
-        <f>IF(G28=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G28, 1) + 23, "000000"),
- IF(G28=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G28, 2) + 11, "000000"),
- IF(G28=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G28, 3) + 12, "000000"),
+      <c r="H29" s="32" t="str">
+        <f>IF(G29=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G29, 1) + 23, "000000"),
+ IF(G29=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G29, 2) + 11, "000000"),
+ IF(G29=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G29, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000019</v>
       </c>
-      <c r="I28" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="I29" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F30" s="31" t="s">
         <v>5182</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G30" s="31">
         <v>1</v>
       </c>
-      <c r="H29" s="2" t="str">
-        <f>IF(G29=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G29, 1) + 23, "000000"),
- IF(G29=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G29, 2) + 11, "000000"),
- IF(G29=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G29, 3) + 12, "000000"),
+      <c r="H30" s="32" t="str">
+        <f>IF(G30=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G30, 1) + 23, "000000"),
+ IF(G30=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G30, 2) + 11, "000000"),
+ IF(G30=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G30, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000037</v>
       </c>
-      <c r="I29" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="I30" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D31" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F31" s="31" t="s">
         <v>5183</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G31" s="31">
         <v>1</v>
       </c>
-      <c r="H30" s="2" t="str">
-        <f>IF(G30=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G30, 1) + 23, "000000"),
- IF(G30=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G30, 2) + 11, "000000"),
- IF(G30=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G30, 3) + 12, "000000"),
+      <c r="H31" s="32" t="str">
+        <f>IF(G31=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G31, 1) + 23, "000000"),
+ IF(G31=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G31, 2) + 11, "000000"),
+ IF(G31=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G31, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000038</v>
       </c>
-      <c r="I30" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="I31" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F32" s="31" t="s">
         <v>5184</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G32" s="31">
         <v>1</v>
       </c>
-      <c r="H31" s="2" t="str">
-        <f>IF(G31=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G31, 1) + 23, "000000"),
- IF(G31=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G31, 2) + 11, "000000"),
- IF(G31=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G31, 3) + 12, "000000"),
+      <c r="H32" s="32" t="str">
+        <f>IF(G32=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G32, 1) + 23, "000000"),
+ IF(G32=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G32, 2) + 11, "000000"),
+ IF(G32=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G32, 3) + 12, "000000"),
  "")))</f>
         <v>PB-000039</v>
       </c>
-      <c r="I31" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="I32" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D33" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F33" s="31" t="s">
         <v>5185</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G33" s="31">
         <v>2</v>
       </c>
-      <c r="H32" s="2" t="str">
-        <f>IF(G32=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G32, 1) + 23, "000000"),
- IF(G32=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G32, 2) + 11, "000000"),
- IF(G32=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G32, 3) + 12, "000000"),
+      <c r="H33" s="32" t="str">
+        <f>IF(G33=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G33, 1) + 23, "000000"),
+ IF(G33=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G33, 2) + 11, "000000"),
+ IF(G33=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G33, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000019</v>
       </c>
-      <c r="I32" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="I33" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="31">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F34" s="31" t="s">
         <v>5186</v>
       </c>
-      <c r="G33" s="3">
+      <c r="G34" s="31">
         <v>3</v>
       </c>
-      <c r="H33" s="2" t="str">
-        <f>IF(G33=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G33, 1) + 23, "000000"),
- IF(G33=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G33, 2) + 11, "000000"),
- IF(G33=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G33, 3) + 12, "000000"),
+      <c r="H34" s="32" t="str">
+        <f>IF(G34=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G34, 1) + 23, "000000"),
+ IF(G34=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G34, 2) + 11, "000000"),
+ IF(G34=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G34, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000020</v>
       </c>
-      <c r="I33" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="I34" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="31" t="s">
         <v>298</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D35" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E35" s="31">
         <v>701812</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F35" s="31" t="s">
         <v>5187</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G35" s="31">
         <v>2</v>
       </c>
-      <c r="H34" s="2" t="str">
-        <f>IF(G34=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G34, 1) + 23, "000000"),
- IF(G34=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G34, 2) + 11, "000000"),
- IF(G34=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G34, 3) + 12, "000000"),
+      <c r="H35" s="32" t="str">
+        <f>IF(G35=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G35, 1) + 23, "000000"),
+ IF(G35=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G35, 2) + 11, "000000"),
+ IF(G35=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G35, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000020</v>
       </c>
-      <c r="I34" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="I35" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="31">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E36" s="31">
         <v>815016</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F36" s="31" t="s">
         <v>5188</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G36" s="31">
         <v>2</v>
       </c>
-      <c r="H35" s="2" t="str">
-        <f>IF(G35=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G35, 1) + 23, "000000"),
- IF(G35=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G35, 2) + 11, "000000"),
- IF(G35=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G35, 3) + 12, "000000"),
+      <c r="H36" s="32" t="str">
+        <f>IF(G36=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G36, 1) + 23, "000000"),
+ IF(G36=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G36, 2) + 11, "000000"),
+ IF(G36=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G36, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000021</v>
       </c>
-      <c r="I35" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="I36" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="31">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="31" t="s">
         <v>300</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E37" s="31">
         <v>161158</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="31" t="s">
         <v>5189</v>
       </c>
-      <c r="G36" s="3">
+      <c r="G37" s="31">
         <v>2</v>
       </c>
-      <c r="H36" s="2" t="str">
-        <f>IF(G36=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G36, 1) + 23, "000000"),
- IF(G36=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G36, 2) + 11, "000000"),
- IF(G36=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G36, 3) + 12, "000000"),
+      <c r="H37" s="32" t="str">
+        <f>IF(G37=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G37, 1) + 23, "000000"),
+ IF(G37=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G37, 2) + 11, "000000"),
+ IF(G37=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G37, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000022</v>
       </c>
-      <c r="I36" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="I37" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="31">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E38" s="31">
         <v>207924</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="31" t="s">
         <v>5190</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G38" s="31">
         <v>2</v>
       </c>
-      <c r="H37" s="2" t="str">
-        <f>IF(G37=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G37, 1) + 23, "000000"),
- IF(G37=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G37, 2) + 11, "000000"),
- IF(G37=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G37, 3) + 12, "000000"),
+      <c r="H38" s="32" t="str">
+        <f>IF(G38=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G38, 1) + 23, "000000"),
+ IF(G38=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G38, 2) + 11, "000000"),
+ IF(G38=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G38, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000023</v>
       </c>
-      <c r="I37" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="I38" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="31">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="31" t="s">
         <v>302</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E39" s="31">
         <v>125635</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="31" t="s">
         <v>5191</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G39" s="31">
         <v>2</v>
       </c>
-      <c r="H38" s="2" t="str">
-        <f>IF(G38=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G38, 1) + 23, "000000"),
- IF(G38=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G38, 2) + 11, "000000"),
- IF(G38=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G38, 3) + 12, "000000"),
+      <c r="H39" s="32" t="str">
+        <f>IF(G39=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G39, 1) + 23, "000000"),
+ IF(G39=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G39, 2) + 11, "000000"),
+ IF(G39=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G39, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000024</v>
       </c>
-      <c r="I38" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="I39" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="31">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="31" t="s">
         <v>303</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E40" s="31">
         <v>207924</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="31" t="s">
         <v>5192</v>
       </c>
-      <c r="G39" s="3">
+      <c r="G40" s="31">
         <v>2</v>
       </c>
-      <c r="H39" s="2" t="str">
-        <f>IF(G39=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G39, 1) + 23, "000000"),
- IF(G39=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G39, 2) + 11, "000000"),
- IF(G39=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G39, 3) + 12, "000000"),
+      <c r="H40" s="32" t="str">
+        <f>IF(G40=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G40, 1) + 23, "000000"),
+ IF(G40=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G40, 2) + 11, "000000"),
+ IF(G40=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G40, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000025</v>
       </c>
-      <c r="I39" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="I40" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="31" t="s">
         <v>277</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E41" s="31">
         <v>207924</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F41" s="31" t="s">
         <v>5193</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G41" s="31">
         <v>2</v>
       </c>
-      <c r="H40" s="2" t="str">
-        <f>IF(G40=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G40, 1) + 23, "000000"),
- IF(G40=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G40, 2) + 11, "000000"),
- IF(G40=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G40, 3) + 12, "000000"),
+      <c r="H41" s="32" t="str">
+        <f>IF(G41=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G41, 1) + 23, "000000"),
+ IF(G41=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G41, 2) + 11, "000000"),
+ IF(G41=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G41, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000026</v>
       </c>
-      <c r="I40" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
+      <c r="I41" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="31">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="31" t="s">
         <v>305</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D42" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E42" s="31">
         <v>880323</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F42" s="31" t="s">
         <v>5194</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G42" s="31">
         <v>2</v>
       </c>
-      <c r="H41" s="2" t="str">
-        <f>IF(G41=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G41, 1) + 23, "000000"),
- IF(G41=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G41, 2) + 11, "000000"),
- IF(G41=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G41, 3) + 12, "000000"),
+      <c r="H42" s="32" t="str">
+        <f>IF(G42=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G42, 1) + 23, "000000"),
+ IF(G42=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G42, 2) + 11, "000000"),
+ IF(G42=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G42, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000027</v>
       </c>
-      <c r="I41" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="I42" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C43" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F43" s="31" t="s">
         <v>5195</v>
       </c>
-      <c r="G42" s="3">
+      <c r="G43" s="31">
         <v>3</v>
       </c>
-      <c r="H42" s="2" t="str">
-        <f>IF(G42=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G42, 1) + 23, "000000"),
- IF(G42=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G42, 2) + 11, "000000"),
- IF(G42=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G42, 3) + 12, "000000"),
+      <c r="H43" s="32" t="str">
+        <f>IF(G43=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G43, 1) + 23, "000000"),
+ IF(G43=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G43, 2) + 11, "000000"),
+ IF(G43=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G43, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000021</v>
       </c>
-      <c r="I42" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="I43" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A44" s="31">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E44" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F44" s="31" t="s">
         <v>5196</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G44" s="31">
         <v>3</v>
       </c>
-      <c r="H43" s="2" t="str">
-        <f>IF(G43=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G43, 1) + 23, "000000"),
- IF(G43=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G43, 2) + 11, "000000"),
- IF(G43=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G43, 3) + 12, "000000"),
+      <c r="H44" s="32" t="str">
+        <f>IF(G44=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G44, 1) + 23, "000000"),
+ IF(G44=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G44, 2) + 11, "000000"),
+ IF(G44=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G44, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000022</v>
       </c>
-      <c r="I43" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="I44" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A45" s="31">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E45" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F45" s="31" t="s">
         <v>5197</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G45" s="31">
         <v>3</v>
       </c>
-      <c r="H44" s="2" t="str">
-        <f>IF(G44=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G44, 1) + 23, "000000"),
- IF(G44=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G44, 2) + 11, "000000"),
- IF(G44=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G44, 3) + 12, "000000"),
+      <c r="H45" s="32" t="str">
+        <f>IF(G45=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G45, 1) + 23, "000000"),
+ IF(G45=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G45, 2) + 11, "000000"),
+ IF(G45=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G45, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000023</v>
       </c>
-      <c r="I44" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="102" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="I45" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="A46" s="31">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B46" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E46" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F46" s="31" t="s">
         <v>5198</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G46" s="31">
         <v>3</v>
       </c>
-      <c r="H45" s="2" t="str">
-        <f>IF(G45=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G45, 1) + 23, "000000"),
- IF(G45=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G45, 2) + 11, "000000"),
- IF(G45=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G45, 3) + 12, "000000"),
+      <c r="H46" s="32" t="str">
+        <f>IF(G46=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G46, 1) + 23, "000000"),
+ IF(G46=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G46, 2) + 11, "000000"),
+ IF(G46=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G46, 3) + 12, "000000"),
  "")))</f>
         <v>MMU-000024</v>
       </c>
-      <c r="I45" s="27" t="s">
-        <v>5346</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="I46" s="34" t="s">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A47" s="31">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C47" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D47" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E47" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F47" s="31" t="s">
         <v>5199</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G47" s="31">
         <v>2</v>
       </c>
-      <c r="H46" s="2" t="str">
-        <f>IF(G46=1, "PB-" &amp; TEXT(COUNTIFS(G$2:G46, 1) + 23, "000000"),
- IF(G46=2, "PBM-" &amp; TEXT(COUNTIFS(G$2:G46, 2) + 11, "000000"),
- IF(G46=3, "MMU-" &amp; TEXT(COUNTIFS(G$2:G46, 3) + 12, "000000"),
+      <c r="H47" s="32" t="str">
+        <f>IF(G47=1, "PB-" &amp; TEXT(COUNTIFS(G$3:G47, 1) + 23, "000000"),
+ IF(G47=2, "PBM-" &amp; TEXT(COUNTIFS(G$3:G47, 2) + 11, "000000"),
+ IF(G47=3, "MMU-" &amp; TEXT(COUNTIFS(G$3:G47, 3) + 12, "000000"),
  "")))</f>
         <v>PBM-000028</v>
       </c>
-      <c r="I46" s="27" t="s">
+      <c r="I47" s="34" t="s">
         <v>5346</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.31496062992125984" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223A2D73-DC32-4B70-A4BC-5814C54A027C}">
-  <sheetPr codeName="Sheet20"/>
+  <sheetPr codeName="Sheet20">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I54"/>
+    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41446,9 +41494,9 @@
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -43234,7 +43282,8 @@
   <conditionalFormatting sqref="I2:I54">
     <cfRule type="uniqueValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.31496062992125984" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -43243,8 +43292,8 @@
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48:I53"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50118,7 +50167,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57997,7 +58046,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58832,7 +58881,7 @@
         <v>5346</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -59657,7 +59706,7 @@
         <v>5346</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
update: requestSoareoartBatch and sparepartUsageBatch
</commit_message>
<xml_diff>
--- a/internal/service/stock/Customer All PB GROUP (Wilayah).xlsx
+++ b/internal/service/stock/Customer All PB GROUP (Wilayah).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\go\src\stock\internal\service\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295C0375-9ADE-424B-A23C-65DDC7ABBB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E1330-C6FF-4174-AE62-F274DEB282AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="13" xr2:uid="{367E69BF-2037-4A2D-B60B-4D531090D608}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="10740" firstSheet="10" activeTab="14" xr2:uid="{367E69BF-2037-4A2D-B60B-4D531090D608}"/>
   </bookViews>
   <sheets>
     <sheet name="Risanto (0) P" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10659" uniqueCount="6882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10689" uniqueCount="6908">
   <si>
     <t>BPR Karya Bakti Sejahtera</t>
   </si>
@@ -20714,6 +20714,84 @@
   </si>
   <si>
     <t>Notaris &amp; PPAT Robby Leo Selamat, SH,.MKn 2</t>
+  </si>
+  <si>
+    <t>W4R8WVZ</t>
+  </si>
+  <si>
+    <t>MUP 15732</t>
+  </si>
+  <si>
+    <t>Fuji Xerox DC-IV 2060CPS</t>
+  </si>
+  <si>
+    <t>Sinar Mas Land Plaza, Menara 2, Lantai 28-30, Jl. MH Thamrin No. 51, Kelurahan Gondangdia, Kecamatan Menteng, Kota Jakarta Pusat</t>
+  </si>
+  <si>
+    <t>Suku Badan Kepegawaian Kota Administrasi Jakarta Selatan</t>
+  </si>
+  <si>
+    <t>Jl. Prapanca Raya No. 9 Kantor Walikota Jakarta Selatan Blok C Lantai 4 Kebayoran Baru, Jakarta Selatan</t>
+  </si>
+  <si>
+    <t>Xerox Apeos/DC - V 5570/5575 FS</t>
+  </si>
+  <si>
+    <t>FCBVKXV</t>
+  </si>
+  <si>
+    <t>PT Jekael Invesco</t>
+  </si>
+  <si>
+    <t>Jl.Gatot Subroto No 38 MenaraBp Jamsostek 2 Lt 2 Menara Selatan Kantor Pengelola</t>
+  </si>
+  <si>
+    <t>Xerox Apeos DC 3370</t>
+  </si>
+  <si>
+    <t>WLHL5TJ</t>
+  </si>
+  <si>
+    <t>Biro Keuangan dan BMN Kementrian Ketenagakerjaan</t>
+  </si>
+  <si>
+    <t>Jl. Gatot Subroto Kav. 51 Gedung A Lt. 3</t>
+  </si>
+  <si>
+    <t>D5DJCIH</t>
+  </si>
+  <si>
+    <t>KJPP Asmawi dan Rekan</t>
+  </si>
+  <si>
+    <t>Ruko Grand Supomo  Jl. Prof Dr Supomo, SH No. 73D Tebet  Jakarta Selatan</t>
+  </si>
+  <si>
+    <t>CHCDJH6</t>
+  </si>
+  <si>
+    <t>PT. Synthesis Karya Pratama (Proyek Gatot Subroto)</t>
+  </si>
+  <si>
+    <t>Synthesis Square Tower II Lantai 8 Jl. Jend Gatot Subroto Kav. 64 No. 177A Jakarta Selatan</t>
+  </si>
+  <si>
+    <t>XWN10078</t>
+  </si>
+  <si>
+    <t>GM7ONZT</t>
+  </si>
+  <si>
+    <t>PT. Synthesis Karya Pratama (Proyek Basura)</t>
+  </si>
+  <si>
+    <t>Bassura City (Marketing Office) Tower Dahlia Jl. Basuki Rahmat No. 1A Jakarta Timur Lt. 1</t>
+  </si>
+  <si>
+    <t>XWN10230</t>
+  </si>
+  <si>
+    <t>122LEXE</t>
   </si>
 </sst>
 </file>
@@ -20904,11 +20982,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -21030,10 +21110,29 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 170" xfId="2" xr:uid="{E6EF9349-1998-4F53-9658-09BA80713D64}"/>
     <cellStyle name="Normal 218" xfId="1" xr:uid="{A6F374D9-7783-4F69-9C99-DA8608612026}"/>
+    <cellStyle name="Normal 96" xfId="3" xr:uid="{3D4433D8-115A-4D1B-BB18-1C6047DDB54C}"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
@@ -21661,8 +21760,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23239,7 +23338,7 @@
   </sheetPr>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -24833,7 +24932,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -26492,7 +26591,7 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -27919,8 +28018,8 @@
   </sheetPr>
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28002,7 +28101,7 @@
         <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>131</v>
+        <v>6883</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5645</v>
@@ -28208,7 +28307,9 @@
       <c r="J8" s="33" t="s">
         <v>6854</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="15" t="s">
+        <v>6882</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -30087,8 +30188,8 @@
   </sheetPr>
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31985,10 +32086,10 @@
   <sheetPr codeName="Sheet15">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33616,33 +33717,126 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+      <c r="A50" s="36">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="36" t="s">
         <v>6844</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="36" t="s">
         <v>6845</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="36" t="s">
         <v>1926</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="36">
         <v>513236</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F50" s="39" t="s">
         <v>6846</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="39">
         <v>3</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" s="39" t="s">
         <v>6847</v>
       </c>
-      <c r="I50" s="25" t="s">
-        <v>5342</v>
-      </c>
+      <c r="I50" s="45" t="s">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="46"/>
+      <c r="B51" s="46" t="s">
+        <v>6894</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>6895</v>
+      </c>
+      <c r="D51" s="46" t="s">
+        <v>1889</v>
+      </c>
+      <c r="E51" s="46">
+        <v>375017</v>
+      </c>
+      <c r="F51" s="46" t="s">
+        <v>6896</v>
+      </c>
+      <c r="G51" s="46">
+        <v>3</v>
+      </c>
+      <c r="H51" s="46"/>
+      <c r="I51" s="43"/>
+    </row>
+    <row r="52" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="46"/>
+      <c r="B52" s="47" t="s">
+        <v>6897</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>6898</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>333</v>
+      </c>
+      <c r="E52" s="49" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F52" s="46" t="s">
+        <v>6899</v>
+      </c>
+      <c r="G52" s="46">
+        <v>2</v>
+      </c>
+      <c r="H52" s="46"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="46" t="s">
+        <v>6900</v>
+      </c>
+      <c r="C53" s="46" t="s">
+        <v>6901</v>
+      </c>
+      <c r="D53" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="E53" s="46" t="s">
+        <v>6902</v>
+      </c>
+      <c r="F53" s="46" t="s">
+        <v>6903</v>
+      </c>
+      <c r="G53" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="46" t="s">
+        <v>6904</v>
+      </c>
+      <c r="C54" s="46" t="s">
+        <v>6905</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>6906</v>
+      </c>
+      <c r="F54" s="46" t="s">
+        <v>6907</v>
+      </c>
+      <c r="G54" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -33661,8 +33855,8 @@
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58728,8 +58922,8 @@
   </sheetPr>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60557,13 +60751,21 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="37"/>
+      <c r="A58" s="35">
+        <v>57</v>
+      </c>
       <c r="B58" s="35" t="s">
         <v>6875</v>
       </c>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
+      <c r="C58" t="s">
+        <v>6885</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6884</v>
+      </c>
+      <c r="E58" s="37">
+        <v>120537</v>
+      </c>
       <c r="F58" s="35" t="s">
         <v>6877</v>
       </c>
@@ -72318,7 +72520,7 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
@@ -73687,10 +73889,10 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75284,7 +75486,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -75317,7 +75519,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -75350,7 +75552,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -75383,7 +75585,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -75416,7 +75618,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -75449,7 +75651,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -75482,7 +75684,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -75515,7 +75717,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -75547,6 +75749,50 @@
       <c r="I56" s="25" t="s">
         <v>5342</v>
       </c>
+    </row>
+    <row r="57" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="A57" s="37"/>
+      <c r="B57" s="35" t="s">
+        <v>6886</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>6887</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>6888</v>
+      </c>
+      <c r="E57" s="37">
+        <v>189167</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>6889</v>
+      </c>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="37"/>
+    </row>
+    <row r="58" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A58" s="37"/>
+      <c r="B58" s="44" t="s">
+        <v>6890</v>
+      </c>
+      <c r="C58" s="44" t="s">
+        <v>6891</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>6892</v>
+      </c>
+      <c r="E58" s="37">
+        <v>125497</v>
+      </c>
+      <c r="F58" s="35" t="s">
+        <v>6893</v>
+      </c>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="43"/>
+      <c r="J58" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -75562,7 +75808,7 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -76643,7 +76889,7 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -80338,7 +80584,7 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>

</xml_diff>